<commit_message>
refactor: optimize model layer and sync related services
</commit_message>
<xml_diff>
--- a/datas/Item.xlsx
+++ b/datas/Item.xlsx
@@ -601,7 +601,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>long</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -1650,7 +1650,6 @@
           <t>icon/doll/cat_01</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
           <t>可爱的小猫玩偶</t>
@@ -1704,7 +1703,6 @@
           <t>icon/doll/dog_01</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
           <t>忠诚的小狗玩偶</t>
@@ -1758,7 +1756,6 @@
           <t>icon/doll/rabbit_01</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
           <t>温柔的兔子玩偶</t>
@@ -1812,7 +1809,6 @@
           <t>icon/doll/fox_01</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
           <t>灵动的狐狸玩偶</t>
@@ -1866,7 +1862,6 @@
           <t>icon/doll/panda_01</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
           <t>憨态可掬的熊猫玩偶</t>
@@ -1920,7 +1915,6 @@
           <t>icon/doll/dragon_01</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
           <t>威风凛凛的幼龙玩偶</t>
@@ -1974,7 +1968,6 @@
           <t>icon/doll/phoenix_01</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
           <t>浴火重生的凤凰玩偶</t>
@@ -2028,7 +2021,6 @@
           <t>icon/doll/knight_01</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
           <t>勇敢的骑士玩偶</t>
@@ -2082,7 +2074,6 @@
           <t>icon/doll/mage_01</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
           <t>神秘的法师玩偶</t>
@@ -2136,7 +2127,6 @@
           <t>icon/doll/archer_01</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
           <t>敏捷的弓箭手玩偶</t>
@@ -2190,7 +2180,6 @@
           <t>icon/doll/paladin_01</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
           <t>圣洁的圣骑士玩偶</t>
@@ -2244,7 +2233,6 @@
           <t>icon/doll/sunflower_01</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
           <t>阳光的向日葵玩偶</t>
@@ -2298,7 +2286,6 @@
           <t>icon/doll/rose_01</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
           <t>优雅的玫瑰玩偶</t>

</xml_diff>